<commit_message>
Excel Aushang Titel korrigiert
</commit_message>
<xml_diff>
--- a/Vortragsmanager/Templates/AushangExcel.xlsx
+++ b/Vortragsmanager/Templates/AushangExcel.xlsx
@@ -492,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1421,6 +1419,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B47:F47"/>
     <mergeCell ref="B83:F83"/>
     <mergeCell ref="B87:F87"/>
     <mergeCell ref="B91:F91"/>
@@ -1430,21 +1443,6 @@
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B75:F75"/>
     <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B39:F39"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.78740157480314965" bottom="0.74803149606299213" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>